<commit_message>
MAJ mapping corps bb8ba8d8f6fde8a744f9d6150934088d548e28fd
</commit_message>
<xml_diff>
--- a/mappingCorps/ig/StructureDefinition-fr-lm-dispositif-medical-entree.xlsx
+++ b/mappingCorps/ig/StructureDefinition-fr-lm-dispositif-medical-entree.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-14T15:34:52+00:00</t>
+    <t>2026-01-16T14:41:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -342,7 +342,7 @@
     <t>fr-lm-dispositif-medical-entree.dispositifMedical</t>
   </si>
   <si>
-    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/document/core/StructureDefinition/FRLMDispositifMedical
+    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/document/core/StructureDefinition/fr-lm-dispositif-medical
 </t>
   </si>
   <si>

</xml_diff>